<commit_message>
Deep Learning -> Cross Validation
</commit_message>
<xml_diff>
--- a/P_Value_AnaCor.xlsx
+++ b/P_Value_AnaCor.xlsx
@@ -460,10 +460,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A2" sqref="A2:A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +503,7 @@
         <v>3.0999999999999999E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -585,7 +586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -602,7 +603,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -630,7 +631,7 @@
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -644,7 +645,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -658,7 +659,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -672,7 +673,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -730,7 +731,7 @@
         <v>6.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -769,7 +770,7 @@
         <v>0.98609999999999998</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -786,7 +787,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -848,7 +849,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E29"/>
+  <autoFilter ref="A1:E29">
+    <filterColumn colId="4">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>